<commit_message>
Update sankey diagram (Finished)
</commit_message>
<xml_diff>
--- a/worldcup-master/data-csv/sankey_diagram.xlsx
+++ b/worldcup-master/data-csv/sankey_diagram.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\World-Cup-2026-\worldcup-master\data-csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8698DC0-3B41-4394-B82C-0FD0FB84538D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49D43E18-C890-4513-9DB1-1D7086880CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" tabRatio="647" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="647" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sankey" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12627" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12616" uniqueCount="411">
   <si>
     <t>stage</t>
   </si>
@@ -1282,9 +1282,6 @@
   <si>
     <t>6</t>
   </si>
-  <si>
-    <t/>
-  </si>
 </sst>
 </file>
 
@@ -1337,18 +1334,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1807,9 +1806,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1871,7 +1867,7 @@
     <tableColumn id="7" xr3:uid="{E6FA5848-DFE7-4FCA-918D-02FFC1BD7CEA}" name="tournament_name"/>
     <tableColumn id="8" xr3:uid="{3903D858-EF71-495D-9418-24E1879F6F12}" name="X"/>
     <tableColumn id="9" xr3:uid="{06E77AC8-689A-4050-A08F-5EAD4942DF40}" name="Multiplier"/>
-    <tableColumn id="10" xr3:uid="{F7C112C5-3E9A-447F-9B4D-D535FD0ED4C1}" name="Y" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{F7C112C5-3E9A-447F-9B4D-D535FD0ED4C1}" name="Y" dataDxfId="0">
       <calculatedColumnFormula>RANDBETWEEN(0,6)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1880,29 +1876,29 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E58355F9-3618-4E87-94B4-1A606FEE2B7C}" name="Table3" displayName="Table3" ref="A1:O171" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O171" xr:uid="{E58355F9-3618-4E87-94B4-1A606FEE2B7C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E58355F9-3618-4E87-94B4-1A606FEE2B7C}" name="Table3" displayName="Table3" ref="A1:O170" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:O170" xr:uid="{E58355F9-3618-4E87-94B4-1A606FEE2B7C}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A157:O168">
-    <sortCondition ref="N2:N171"/>
-    <sortCondition ref="E2:E171"/>
-    <sortCondition ref="I2:I171"/>
+    <sortCondition ref="N2:N170"/>
+    <sortCondition ref="E2:E170"/>
+    <sortCondition ref="I2:I170"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{BF4D807A-CA7A-4DC7-AB50-F97393DD939E}" name="team_name" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7F4F1EBA-6643-4BCF-A58A-95123A7F3023}" name="team_region" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{B6A4B3B8-61E8-4FD0-B8D3-7CA4886467D1}" name="team_confederation_code" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{A5B3FF21-01FE-4316-A843-7062B8B96243}" name="tournament_id" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{F18002B8-4212-4513-8459-B07079AFB507}" name="team_code" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{1592D8F2-6B50-4A85-8E4F-3176876730C3}" name="tournament_name" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{0225DF71-5C31-4DC6-8337-F33877215076}" name="X" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{5544A805-73BE-4AC8-BEFD-8EA711F8FE6B}" name="Multiplier" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{E302AAE7-1F3F-4B80-A0FF-632EF8321CB6}" name="Y" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{86EA23E1-ED65-4375-8184-B5DAA874A3F5}" name="farthest_stage_" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{DB3B3828-1975-4C87-A0FF-32F7B511F818}" name="grouped_farthest_stage" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{F76D4808-B140-4029-A49A-23E8145CF64B}" name="farthest_stage" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{6AEE708D-432B-4ADF-B1FB-6A9D22EE6EBF}" name="Year_WC" dataDxfId="2"/>
-    <tableColumn id="14" xr3:uid="{984DF2AC-EB67-4FBB-892A-A67E0B270B4E}" name="stage_rank" dataDxfId="1"/>
-    <tableColumn id="15" xr3:uid="{D4966489-9649-49AB-B522-4619F9643CD4}" name="team_id" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BF4D807A-CA7A-4DC7-AB50-F97393DD939E}" name="team_name" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{7F4F1EBA-6643-4BCF-A58A-95123A7F3023}" name="team_region" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{B6A4B3B8-61E8-4FD0-B8D3-7CA4886467D1}" name="team_confederation_code" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{A5B3FF21-01FE-4316-A843-7062B8B96243}" name="tournament_id" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{F18002B8-4212-4513-8459-B07079AFB507}" name="team_code" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{1592D8F2-6B50-4A85-8E4F-3176876730C3}" name="tournament_name" dataDxfId="10"/>
+    <tableColumn id="7" xr3:uid="{0225DF71-5C31-4DC6-8337-F33877215076}" name="X" dataDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{5544A805-73BE-4AC8-BEFD-8EA711F8FE6B}" name="Multiplier" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{E302AAE7-1F3F-4B80-A0FF-632EF8321CB6}" name="Y" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{86EA23E1-ED65-4375-8184-B5DAA874A3F5}" name="farthest_stage_" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{DB3B3828-1975-4C87-A0FF-32F7B511F818}" name="grouped_farthest_stage" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{F76D4808-B140-4029-A49A-23E8145CF64B}" name="farthest_stage" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{6AEE708D-432B-4ADF-B1FB-6A9D22EE6EBF}" name="Year_WC" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{984DF2AC-EB67-4FBB-892A-A67E0B270B4E}" name="stage_rank" dataDxfId="2"/>
+    <tableColumn id="15" xr3:uid="{D4966489-9649-49AB-B522-4619F9643CD4}" name="team_id" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -10446,10 +10442,10 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:O171"/>
+  <dimension ref="A1:O170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D159" workbookViewId="0">
-      <selection activeCell="G169" sqref="G169"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10556,7 +10552,7 @@
       <c r="M2" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -10603,7 +10599,7 @@
       <c r="M3" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -10650,7 +10646,7 @@
       <c r="M4" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="N4" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -10697,7 +10693,7 @@
       <c r="M5" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="N5" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O5" s="3" t="s">
@@ -10744,7 +10740,7 @@
       <c r="M6" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O6" s="3" t="s">
@@ -10791,7 +10787,7 @@
       <c r="M7" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O7" s="3" t="s">
@@ -10838,7 +10834,7 @@
       <c r="M8" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O8" s="3" t="s">
@@ -10885,7 +10881,7 @@
       <c r="M9" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O9" s="3" t="s">
@@ -10932,7 +10928,7 @@
       <c r="M10" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O10" s="3" t="s">
@@ -10979,7 +10975,7 @@
       <c r="M11" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O11" s="3" t="s">
@@ -11026,7 +11022,7 @@
       <c r="M12" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O12" s="3" t="s">
@@ -11073,7 +11069,7 @@
       <c r="M13" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O13" s="3" t="s">
@@ -11120,7 +11116,7 @@
       <c r="M14" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O14" s="3" t="s">
@@ -11167,7 +11163,7 @@
       <c r="M15" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O15" s="3" t="s">
@@ -11214,7 +11210,7 @@
       <c r="M16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O16" s="3" t="s">
@@ -11261,7 +11257,7 @@
       <c r="M17" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O17" s="3" t="s">
@@ -11308,7 +11304,7 @@
       <c r="M18" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O18" s="3" t="s">
@@ -11355,7 +11351,7 @@
       <c r="M19" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O19" s="3" t="s">
@@ -11402,7 +11398,7 @@
       <c r="M20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="N20" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O20" s="3" t="s">
@@ -11449,7 +11445,7 @@
       <c r="M21" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N21" s="5" t="s">
+      <c r="N21" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O21" s="3" t="s">
@@ -11496,7 +11492,7 @@
       <c r="M22" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N22" s="5" t="s">
+      <c r="N22" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O22" s="3" t="s">
@@ -11543,7 +11539,7 @@
       <c r="M23" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="N23" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O23" s="3" t="s">
@@ -11590,7 +11586,7 @@
       <c r="M24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="N24" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O24" s="3" t="s">
@@ -11637,7 +11633,7 @@
       <c r="M25" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="N25" s="5" t="s">
+      <c r="N25" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O25" s="3" t="s">
@@ -11684,7 +11680,7 @@
       <c r="M26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O26" s="3" t="s">
@@ -11731,7 +11727,7 @@
       <c r="M27" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N27" s="5" t="s">
+      <c r="N27" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O27" s="3" t="s">
@@ -11778,7 +11774,7 @@
       <c r="M28" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N28" s="5" t="s">
+      <c r="N28" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O28" s="3" t="s">
@@ -11825,7 +11821,7 @@
       <c r="M29" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="N29" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O29" s="3" t="s">
@@ -11872,7 +11868,7 @@
       <c r="M30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="N30" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O30" s="3" t="s">
@@ -11919,7 +11915,7 @@
       <c r="M31" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N31" s="5" t="s">
+      <c r="N31" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O31" s="3" t="s">
@@ -11966,7 +11962,7 @@
       <c r="M32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N32" s="5" t="s">
+      <c r="N32" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O32" s="3" t="s">
@@ -12013,7 +12009,7 @@
       <c r="M33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N33" s="5" t="s">
+      <c r="N33" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O33" s="3" t="s">
@@ -12060,7 +12056,7 @@
       <c r="M34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="N34" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O34" s="3" t="s">
@@ -12107,7 +12103,7 @@
       <c r="M35" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N35" s="5" t="s">
+      <c r="N35" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O35" s="3" t="s">
@@ -12154,7 +12150,7 @@
       <c r="M36" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N36" s="5" t="s">
+      <c r="N36" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O36" s="3" t="s">
@@ -12201,7 +12197,7 @@
       <c r="M37" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="5" t="s">
+      <c r="N37" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O37" s="3" t="s">
@@ -12248,7 +12244,7 @@
       <c r="M38" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N38" s="5" t="s">
+      <c r="N38" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O38" s="3" t="s">
@@ -12295,7 +12291,7 @@
       <c r="M39" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N39" s="5" t="s">
+      <c r="N39" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O39" s="3" t="s">
@@ -12342,7 +12338,7 @@
       <c r="M40" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="N40" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O40" s="3" t="s">
@@ -12389,7 +12385,7 @@
       <c r="M41" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N41" s="5" t="s">
+      <c r="N41" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O41" s="3" t="s">
@@ -12436,7 +12432,7 @@
       <c r="M42" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N42" s="5" t="s">
+      <c r="N42" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O42" s="3" t="s">
@@ -12483,7 +12479,7 @@
       <c r="M43" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N43" s="5" t="s">
+      <c r="N43" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O43" s="3" t="s">
@@ -12530,7 +12526,7 @@
       <c r="M44" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N44" s="5" t="s">
+      <c r="N44" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O44" s="3" t="s">
@@ -12577,7 +12573,7 @@
       <c r="M45" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N45" s="5" t="s">
+      <c r="N45" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O45" s="3" t="s">
@@ -12624,7 +12620,7 @@
       <c r="M46" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N46" s="5" t="s">
+      <c r="N46" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O46" s="3" t="s">
@@ -12671,7 +12667,7 @@
       <c r="M47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N47" s="5" t="s">
+      <c r="N47" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O47" s="3" t="s">
@@ -12718,7 +12714,7 @@
       <c r="M48" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N48" s="5" t="s">
+      <c r="N48" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O48" s="3" t="s">
@@ -12765,7 +12761,7 @@
       <c r="M49" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N49" s="5" t="s">
+      <c r="N49" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O49" s="3" t="s">
@@ -12812,7 +12808,7 @@
       <c r="M50" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N50" s="5" t="s">
+      <c r="N50" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O50" s="3" t="s">
@@ -12859,7 +12855,7 @@
       <c r="M51" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N51" s="5" t="s">
+      <c r="N51" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O51" s="3" t="s">
@@ -12906,7 +12902,7 @@
       <c r="M52" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N52" s="5" t="s">
+      <c r="N52" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O52" s="3" t="s">
@@ -12953,7 +12949,7 @@
       <c r="M53" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N53" s="5" t="s">
+      <c r="N53" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O53" s="3" t="s">
@@ -13000,7 +12996,7 @@
       <c r="M54" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N54" s="5" t="s">
+      <c r="N54" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O54" s="3" t="s">
@@ -13047,7 +13043,7 @@
       <c r="M55" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N55" s="5" t="s">
+      <c r="N55" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O55" s="3" t="s">
@@ -13094,7 +13090,7 @@
       <c r="M56" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N56" s="5" t="s">
+      <c r="N56" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O56" s="3" t="s">
@@ -13141,7 +13137,7 @@
       <c r="M57" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N57" s="5" t="s">
+      <c r="N57" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O57" s="3" t="s">
@@ -13188,7 +13184,7 @@
       <c r="M58" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N58" s="5" t="s">
+      <c r="N58" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O58" s="3" t="s">
@@ -13235,7 +13231,7 @@
       <c r="M59" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N59" s="5" t="s">
+      <c r="N59" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O59" s="3" t="s">
@@ -13282,7 +13278,7 @@
       <c r="M60" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N60" s="5" t="s">
+      <c r="N60" s="3" t="s">
         <v>405</v>
       </c>
       <c r="O60" s="3" t="s">
@@ -13329,7 +13325,7 @@
       <c r="M61" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N61" s="5" t="s">
+      <c r="N61" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O61" s="3" t="s">
@@ -13376,7 +13372,7 @@
       <c r="M62" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N62" s="5" t="s">
+      <c r="N62" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O62" s="3" t="s">
@@ -13423,7 +13419,7 @@
       <c r="M63" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N63" s="5" t="s">
+      <c r="N63" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O63" s="3" t="s">
@@ -13470,7 +13466,7 @@
       <c r="M64" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N64" s="5" t="s">
+      <c r="N64" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O64" s="3" t="s">
@@ -13517,7 +13513,7 @@
       <c r="M65" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N65" s="5" t="s">
+      <c r="N65" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O65" s="3" t="s">
@@ -13564,7 +13560,7 @@
       <c r="M66" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N66" s="5" t="s">
+      <c r="N66" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O66" s="3" t="s">
@@ -13611,7 +13607,7 @@
       <c r="M67" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N67" s="5" t="s">
+      <c r="N67" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O67" s="3" t="s">
@@ -13658,7 +13654,7 @@
       <c r="M68" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="N68" s="5" t="s">
+      <c r="N68" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O68" s="3" t="s">
@@ -13705,7 +13701,7 @@
       <c r="M69" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N69" s="5" t="s">
+      <c r="N69" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O69" s="3" t="s">
@@ -13752,7 +13748,7 @@
       <c r="M70" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N70" s="5" t="s">
+      <c r="N70" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O70" s="3" t="s">
@@ -13799,7 +13795,7 @@
       <c r="M71" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N71" s="5" t="s">
+      <c r="N71" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O71" s="3" t="s">
@@ -13846,7 +13842,7 @@
       <c r="M72" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N72" s="5" t="s">
+      <c r="N72" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O72" s="3" t="s">
@@ -13893,7 +13889,7 @@
       <c r="M73" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N73" s="5" t="s">
+      <c r="N73" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O73" s="3" t="s">
@@ -13940,7 +13936,7 @@
       <c r="M74" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N74" s="5" t="s">
+      <c r="N74" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O74" s="3" t="s">
@@ -13987,7 +13983,7 @@
       <c r="M75" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N75" s="5" t="s">
+      <c r="N75" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O75" s="3" t="s">
@@ -14034,7 +14030,7 @@
       <c r="M76" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N76" s="5" t="s">
+      <c r="N76" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O76" s="3" t="s">
@@ -14081,7 +14077,7 @@
       <c r="M77" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N77" s="5" t="s">
+      <c r="N77" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O77" s="3" t="s">
@@ -14128,7 +14124,7 @@
       <c r="M78" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N78" s="5" t="s">
+      <c r="N78" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O78" s="3" t="s">
@@ -14175,7 +14171,7 @@
       <c r="M79" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N79" s="5" t="s">
+      <c r="N79" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O79" s="3" t="s">
@@ -14222,7 +14218,7 @@
       <c r="M80" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N80" s="5" t="s">
+      <c r="N80" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O80" s="3" t="s">
@@ -14269,7 +14265,7 @@
       <c r="M81" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N81" s="5" t="s">
+      <c r="N81" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O81" s="3" t="s">
@@ -14316,7 +14312,7 @@
       <c r="M82" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N82" s="5" t="s">
+      <c r="N82" s="3" t="s">
         <v>406</v>
       </c>
       <c r="O82" s="3" t="s">
@@ -14363,7 +14359,7 @@
       <c r="M83" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="N83" s="5" t="s">
+      <c r="N83" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O83" s="3" t="s">
@@ -14410,7 +14406,7 @@
       <c r="M84" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="N84" s="5" t="s">
+      <c r="N84" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O84" s="3" t="s">
@@ -14457,7 +14453,7 @@
       <c r="M85" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N85" s="5" t="s">
+      <c r="N85" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O85" s="3" t="s">
@@ -14504,7 +14500,7 @@
       <c r="M86" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N86" s="5" t="s">
+      <c r="N86" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O86" s="3" t="s">
@@ -14551,7 +14547,7 @@
       <c r="M87" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N87" s="5" t="s">
+      <c r="N87" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O87" s="3" t="s">
@@ -14598,7 +14594,7 @@
       <c r="M88" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N88" s="5" t="s">
+      <c r="N88" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O88" s="3" t="s">
@@ -14645,7 +14641,7 @@
       <c r="M89" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N89" s="5" t="s">
+      <c r="N89" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O89" s="3" t="s">
@@ -14692,7 +14688,7 @@
       <c r="M90" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N90" s="5" t="s">
+      <c r="N90" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O90" s="3" t="s">
@@ -14739,7 +14735,7 @@
       <c r="M91" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N91" s="5" t="s">
+      <c r="N91" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O91" s="3" t="s">
@@ -14786,7 +14782,7 @@
       <c r="M92" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="N92" s="5" t="s">
+      <c r="N92" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O92" s="3" t="s">
@@ -14833,7 +14829,7 @@
       <c r="M93" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N93" s="5" t="s">
+      <c r="N93" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O93" s="3" t="s">
@@ -14880,7 +14876,7 @@
       <c r="M94" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="N94" s="5" t="s">
+      <c r="N94" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O94" s="3" t="s">
@@ -14927,7 +14923,7 @@
       <c r="M95" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N95" s="5" t="s">
+      <c r="N95" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O95" s="3" t="s">
@@ -14974,7 +14970,7 @@
       <c r="M96" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N96" s="5" t="s">
+      <c r="N96" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O96" s="3" t="s">
@@ -15021,7 +15017,7 @@
       <c r="M97" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N97" s="5" t="s">
+      <c r="N97" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O97" s="3" t="s">
@@ -15068,7 +15064,7 @@
       <c r="M98" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="N98" s="5" t="s">
+      <c r="N98" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O98" s="3" t="s">
@@ -15115,7 +15111,7 @@
       <c r="M99" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N99" s="5" t="s">
+      <c r="N99" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O99" s="3" t="s">
@@ -15162,7 +15158,7 @@
       <c r="M100" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N100" s="5" t="s">
+      <c r="N100" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O100" s="3" t="s">
@@ -15209,7 +15205,7 @@
       <c r="M101" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N101" s="5" t="s">
+      <c r="N101" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O101" s="3" t="s">
@@ -15256,7 +15252,7 @@
       <c r="M102" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N102" s="5" t="s">
+      <c r="N102" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O102" s="3" t="s">
@@ -15303,7 +15299,7 @@
       <c r="M103" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N103" s="5" t="s">
+      <c r="N103" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O103" s="3" t="s">
@@ -15350,7 +15346,7 @@
       <c r="M104" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N104" s="5" t="s">
+      <c r="N104" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O104" s="3" t="s">
@@ -15397,7 +15393,7 @@
       <c r="M105" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N105" s="5" t="s">
+      <c r="N105" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O105" s="3" t="s">
@@ -15444,7 +15440,7 @@
       <c r="M106" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N106" s="5" t="s">
+      <c r="N106" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O106" s="3" t="s">
@@ -15491,7 +15487,7 @@
       <c r="M107" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N107" s="5" t="s">
+      <c r="N107" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O107" s="3" t="s">
@@ -15538,7 +15534,7 @@
       <c r="M108" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N108" s="5" t="s">
+      <c r="N108" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O108" s="3" t="s">
@@ -15585,7 +15581,7 @@
       <c r="M109" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N109" s="5" t="s">
+      <c r="N109" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O109" s="3" t="s">
@@ -15632,7 +15628,7 @@
       <c r="M110" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N110" s="5" t="s">
+      <c r="N110" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O110" s="3" t="s">
@@ -15679,7 +15675,7 @@
       <c r="M111" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N111" s="5" t="s">
+      <c r="N111" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O111" s="3" t="s">
@@ -15726,7 +15722,7 @@
       <c r="M112" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N112" s="5" t="s">
+      <c r="N112" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O112" s="3" t="s">
@@ -15773,7 +15769,7 @@
       <c r="M113" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N113" s="5" t="s">
+      <c r="N113" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O113" s="3" t="s">
@@ -15820,7 +15816,7 @@
       <c r="M114" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N114" s="5" t="s">
+      <c r="N114" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O114" s="3" t="s">
@@ -15867,7 +15863,7 @@
       <c r="M115" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N115" s="5" t="s">
+      <c r="N115" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O115" s="3" t="s">
@@ -15914,7 +15910,7 @@
       <c r="M116" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N116" s="5" t="s">
+      <c r="N116" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O116" s="3" t="s">
@@ -15961,7 +15957,7 @@
       <c r="M117" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N117" s="5" t="s">
+      <c r="N117" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O117" s="3" t="s">
@@ -16008,7 +16004,7 @@
       <c r="M118" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N118" s="5" t="s">
+      <c r="N118" s="3" t="s">
         <v>407</v>
       </c>
       <c r="O118" s="3" t="s">
@@ -16055,7 +16051,7 @@
       <c r="M119" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="N119" s="5" t="s">
+      <c r="N119" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O119" s="3" t="s">
@@ -16102,7 +16098,7 @@
       <c r="M120" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="N120" s="5" t="s">
+      <c r="N120" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O120" s="3" t="s">
@@ -16149,7 +16145,7 @@
       <c r="M121" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N121" s="5" t="s">
+      <c r="N121" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O121" s="3" t="s">
@@ -16196,7 +16192,7 @@
       <c r="M122" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N122" s="5" t="s">
+      <c r="N122" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O122" s="3" t="s">
@@ -16243,7 +16239,7 @@
       <c r="M123" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N123" s="5" t="s">
+      <c r="N123" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O123" s="3" t="s">
@@ -16290,7 +16286,7 @@
       <c r="M124" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N124" s="5" t="s">
+      <c r="N124" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O124" s="3" t="s">
@@ -16337,7 +16333,7 @@
       <c r="M125" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N125" s="5" t="s">
+      <c r="N125" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O125" s="3" t="s">
@@ -16384,7 +16380,7 @@
       <c r="M126" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N126" s="5" t="s">
+      <c r="N126" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O126" s="3" t="s">
@@ -16431,7 +16427,7 @@
       <c r="M127" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N127" s="5" t="s">
+      <c r="N127" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O127" s="3" t="s">
@@ -16478,7 +16474,7 @@
       <c r="M128" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N128" s="5" t="s">
+      <c r="N128" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O128" s="3" t="s">
@@ -16525,7 +16521,7 @@
       <c r="M129" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N129" s="5" t="s">
+      <c r="N129" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O129" s="3" t="s">
@@ -16572,7 +16568,7 @@
       <c r="M130" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N130" s="5" t="s">
+      <c r="N130" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O130" s="3" t="s">
@@ -16619,7 +16615,7 @@
       <c r="M131" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N131" s="5" t="s">
+      <c r="N131" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O131" s="3" t="s">
@@ -16666,7 +16662,7 @@
       <c r="M132" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N132" s="5" t="s">
+      <c r="N132" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O132" s="3" t="s">
@@ -16713,7 +16709,7 @@
       <c r="M133" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N133" s="5" t="s">
+      <c r="N133" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O133" s="3" t="s">
@@ -16760,7 +16756,7 @@
       <c r="M134" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="N134" s="5" t="s">
+      <c r="N134" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O134" s="3" t="s">
@@ -16807,7 +16803,7 @@
       <c r="M135" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N135" s="5" t="s">
+      <c r="N135" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O135" s="3" t="s">
@@ -16854,7 +16850,7 @@
       <c r="M136" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N136" s="5" t="s">
+      <c r="N136" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O136" s="3" t="s">
@@ -16901,7 +16897,7 @@
       <c r="M137" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N137" s="5" t="s">
+      <c r="N137" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O137" s="3" t="s">
@@ -16948,7 +16944,7 @@
       <c r="M138" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="N138" s="5" t="s">
+      <c r="N138" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O138" s="3" t="s">
@@ -16995,7 +16991,7 @@
       <c r="M139" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N139" s="5" t="s">
+      <c r="N139" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O139" s="3" t="s">
@@ -17042,7 +17038,7 @@
       <c r="M140" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N140" s="5" t="s">
+      <c r="N140" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O140" s="3" t="s">
@@ -17089,7 +17085,7 @@
       <c r="M141" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N141" s="5" t="s">
+      <c r="N141" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O141" s="3" t="s">
@@ -17136,7 +17132,7 @@
       <c r="M142" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N142" s="5" t="s">
+      <c r="N142" s="3" t="s">
         <v>408</v>
       </c>
       <c r="O142" s="3" t="s">
@@ -17183,7 +17179,7 @@
       <c r="M143" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N143" s="5" t="s">
+      <c r="N143" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O143" s="3" t="s">
@@ -17230,7 +17226,7 @@
       <c r="M144" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="N144" s="5" t="s">
+      <c r="N144" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O144" s="3" t="s">
@@ -17277,7 +17273,7 @@
       <c r="M145" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N145" s="5" t="s">
+      <c r="N145" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O145" s="3" t="s">
@@ -17324,7 +17320,7 @@
       <c r="M146" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N146" s="5" t="s">
+      <c r="N146" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O146" s="3" t="s">
@@ -17371,7 +17367,7 @@
       <c r="M147" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="N147" s="5" t="s">
+      <c r="N147" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O147" s="3" t="s">
@@ -17418,7 +17414,7 @@
       <c r="M148" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="N148" s="5" t="s">
+      <c r="N148" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O148" s="3" t="s">
@@ -17465,7 +17461,7 @@
       <c r="M149" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N149" s="5" t="s">
+      <c r="N149" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O149" s="3" t="s">
@@ -17512,7 +17508,7 @@
       <c r="M150" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N150" s="5" t="s">
+      <c r="N150" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O150" s="3" t="s">
@@ -17559,7 +17555,7 @@
       <c r="M151" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N151" s="5" t="s">
+      <c r="N151" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O151" s="3" t="s">
@@ -17606,7 +17602,7 @@
       <c r="M152" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="N152" s="5" t="s">
+      <c r="N152" s="3" t="s">
         <v>409</v>
       </c>
       <c r="O152" s="3" t="s">
@@ -17653,7 +17649,7 @@
       <c r="M153" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N153" s="5" t="s">
+      <c r="N153" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O153" s="3" t="s">
@@ -17700,7 +17696,7 @@
       <c r="M154" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="N154" s="5" t="s">
+      <c r="N154" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O154" s="3" t="s">
@@ -17747,7 +17743,7 @@
       <c r="M155" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N155" s="5" t="s">
+      <c r="N155" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O155" s="3" t="s">
@@ -17794,7 +17790,7 @@
       <c r="M156" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="N156" s="5" t="s">
+      <c r="N156" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O156" s="3" t="s">
@@ -17841,7 +17837,7 @@
       <c r="M157" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N157" s="5">
+      <c r="N157" s="3">
         <v>6</v>
       </c>
       <c r="O157" s="3" t="s">
@@ -17888,7 +17884,7 @@
       <c r="M158" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N158" s="5">
+      <c r="N158" s="3">
         <v>6</v>
       </c>
       <c r="O158" s="3" t="s">
@@ -17935,7 +17931,7 @@
       <c r="M159" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N159" s="5" t="s">
+      <c r="N159" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O159" s="3" t="s">
@@ -17982,7 +17978,7 @@
       <c r="M160" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="N160" s="5" t="s">
+      <c r="N160" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O160" s="3" t="s">
@@ -18029,7 +18025,7 @@
       <c r="M161" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N161" s="5" t="s">
+      <c r="N161" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O161" s="3" t="s">
@@ -18076,7 +18072,7 @@
       <c r="M162" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="N162" s="5" t="s">
+      <c r="N162" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O162" s="3" t="s">
@@ -18123,7 +18119,7 @@
       <c r="M163" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N163" s="5" t="s">
+      <c r="N163" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O163" s="3" t="s">
@@ -18170,7 +18166,7 @@
       <c r="M164" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="N164" s="5" t="s">
+      <c r="N164" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O164" s="3" t="s">
@@ -18217,7 +18213,7 @@
       <c r="M165" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N165" s="5" t="s">
+      <c r="N165" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O165" s="3" t="s">
@@ -18264,7 +18260,7 @@
       <c r="M166" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="N166" s="5" t="s">
+      <c r="N166" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O166" s="3" t="s">
@@ -18311,7 +18307,7 @@
       <c r="M167" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N167" s="5" t="s">
+      <c r="N167" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O167" s="3" t="s">
@@ -18358,7 +18354,7 @@
       <c r="M168" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="N168" s="5" t="s">
+      <c r="N168" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O168" s="3" t="s">
@@ -18405,7 +18401,7 @@
       <c r="M169" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N169" s="5" t="s">
+      <c r="N169" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O169" s="3" t="s">
@@ -18452,58 +18448,11 @@
       <c r="M170" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="N170" s="5" t="s">
+      <c r="N170" s="3" t="s">
         <v>410</v>
       </c>
       <c r="O170" s="3" t="s">
         <v>394</v>
-      </c>
-    </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A171" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="C171" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="D171" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G171" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="H171" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="I171" s="4">
-        <v>0</v>
-      </c>
-      <c r="J171" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K171" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="L171" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="M171" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="N171" s="5">
-        <v>1</v>
-      </c>
-      <c r="O171" s="3" t="s">
-        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>